<commit_message>
Ready to go! Mungbeans in Stilettos!
</commit_message>
<xml_diff>
--- a/Tests/UnderReview/Mungbean/ObservedData.xlsx
+++ b/Tests/UnderReview/Mungbean/ObservedData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pas075\Documents\ApsimX\Tests\UnderReview\Mungbean\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22110A2F-639E-48C7-830B-D89CC43A7A9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{988AE31C-75DA-40D9-BEE6-7DF199F380AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28035" windowHeight="16440" activeTab="1" xr2:uid="{9FA297CA-29B6-4A83-B4E5-4BA784BC781A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28065" windowHeight="16440" xr2:uid="{9FA297CA-29B6-4A83-B4E5-4BA784BC781A}"/>
   </bookViews>
   <sheets>
     <sheet name="PlantBiomassObserved" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">NitrogenObserved!$A$1:$AC$352</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">PhenologyObserved!$A$1:$N$831</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">PlantBiomassObserved!$A$1:$W$451</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">SoilWaterObserved!$A$1:$T$84</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -1183,8 +1184,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98D7DBC0-8FFD-4004-98F0-2F6AD6B427E8}">
   <dimension ref="A1:W451"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B101" sqref="B101"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2463,7 +2464,7 @@
         <v>26</v>
       </c>
       <c r="F67">
-        <v>587</v>
+        <v>866</v>
       </c>
       <c r="H67">
         <v>2930</v>
@@ -2570,7 +2571,7 @@
         <v>26</v>
       </c>
       <c r="F74">
-        <v>866</v>
+        <v>587</v>
       </c>
       <c r="H74">
         <v>2810</v>
@@ -12386,7 +12387,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DBEDAAD-4E07-4543-B9D3-A0ED902D4CED}">
   <dimension ref="A1:AC352"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="U2" sqref="U2"/>
     </sheetView>
   </sheetViews>

</xml_diff>